<commit_message>
correctifs pour publier 82d1e725c017ed9a73c92a83cf7f734ebfc1ba31
</commit_message>
<xml_diff>
--- a/Publication-Release4.0.2-ballot-3/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/Publication-Release4.0.2-ballot-3/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -45,7 +45,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>active</t>
+    <t>draft</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-17T14:29:26+00:00</t>
+    <t>2024-04-18T08:51:23+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>